<commit_message>
update event tables - update ER
</commit_message>
<xml_diff>
--- a/Entities/DB_Entities.xlsx
+++ b/Entities/DB_Entities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masoud\Desktop\salaam\Tiwall\Entities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B3FAD-59B2-495A-A698-9B2F1CB6C428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85C4C1F-11DE-444D-B343-94BA22D6B443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="90">
   <si>
     <t>Entity/Feature</t>
   </si>
@@ -947,7 +947,7 @@
   <dimension ref="A1:AF1022"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1032,29 +1032,16 @@
         <v>8</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>10</v>
+      <c r="J2" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
       <c r="Q2" s="8"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
@@ -1113,8 +1100,12 @@
       <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="7"/>
@@ -1187,7 +1178,9 @@
       <c r="C6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1261,8 +1254,12 @@
       <c r="C8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -1335,8 +1332,12 @@
       <c r="C10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -1409,10 +1410,18 @@
       <c r="C12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="H12" s="8"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -1483,9 +1492,15 @@
       <c r="C14" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -1557,9 +1572,15 @@
       <c r="C16" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="7"/>
+      <c r="D16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>

</xml_diff>

<commit_message>
some bugs fixed in concert table
</commit_message>
<xml_diff>
--- a/Entities/DB_Entities.xlsx
+++ b/Entities/DB_Entities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masoud\Desktop\salaam\Tiwall\Entities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85C4C1F-11DE-444D-B343-94BA22D6B443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F633384-5A1C-4517-B668-0CFBA50E216A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:AF1022"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
events added to relative tables, inserted new casts and cast_occupation
</commit_message>
<xml_diff>
--- a/Entities/DB_Entities.xlsx
+++ b/Entities/DB_Entities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masoud\Desktop\salaam\Tiwall\Entities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F633384-5A1C-4517-B668-0CFBA50E216A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9092030D-BFEA-423A-9834-9740C9C1A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
   <si>
     <t>Entity/Feature</t>
   </si>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1422,7 +1422,9 @@
       <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>

</xml_diff>